<commit_message>
Add Generated Files to a folder
</commit_message>
<xml_diff>
--- a/Audio Sequence.xlsx
+++ b/Audio Sequence.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -28,25 +28,19 @@
     <t xml:space="preserve">Text</t>
   </si>
   <si>
-    <t xml:space="preserve">Welcome to this tutorial video which teaches you how to design a PCB using Easy E D A.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy E D A is a free to use, and you can create PCBs on this software for your projects. There is no need to install anything, it runs in a modern browser.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I already have an account, so that is what I am using. You can pause the video here, go ahead and create an account, and come back here to continue.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you are logged in, you can access the PCB editor by clicking here. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can access your past projects here in the project explorer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Let us go ahead and create a new project.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I want to create a PCB for an E S P zero one module, which will send me a notification when two pins on the E S P zero one are connected together. Let us see how to do that. </t>
+    <t xml:space="preserve">Let us now perform the activity on the breadboard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We will build the same circuit that we create on tinker CAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So now  we have the same components that we use in our tinkercad simulation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A breadboard, three resistors, two of one kiloohm each and one of ten kiloohm. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A 9 volts battery, a digital multimeter.</t>
   </si>
 </sst>
 </file>
@@ -176,10 +170,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,22 +231,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>82</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>93</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>